<commit_message>
Fixed Parsing errors with naming WS naming conflicts
Can now parse when WS names are ‘Data’ or if there are some weird
spacing. Successfully parsed all 3 example folders Africa, O2KLR, and
SAm. All CSV and JSON output is perfect.
</commit_message>
<xml_diff>
--- a/Parser/xlsfiles/2014-2kphase2-Arctic1147Bonnet2010.xlsx
+++ b/Parser/xlsfiles/2014-2kphase2-Arctic1147Bonnet2010.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="24460" windowHeight="15120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="2" r:id="rId1"/>
-    <sheet name="Chronology" sheetId="7" r:id="rId2"/>
-    <sheet name="Data (QC)" sheetId="3" r:id="rId3"/>
-    <sheet name="ProxyList" sheetId="5" state="hidden" r:id="rId4"/>
-    <sheet name="Data (original)" sheetId="9" r:id="rId5"/>
-    <sheet name="About" sheetId="8" r:id="rId6"/>
+    <sheet name="About" sheetId="8" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Chronology" sheetId="7" r:id="rId3"/>
+    <sheet name="Data (QC)" sheetId="3" r:id="rId4"/>
+    <sheet name="ProxyList" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="Data (original)" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="ProxyList">ProxyList!$A$4:$A$23</definedName>
     <definedName name="ProxyList2">ProxyList!$A$3:$A$23</definedName>
   </definedNames>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -764,7 +764,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1339,19 +1339,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="69.5" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="69.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="8" customFormat="1">
@@ -1405,8 +1476,8 @@
         <v>192</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1"/>
-    <row r="9" spans="1:3" ht="16" thickTop="1" thickBot="1">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1"/>
+    <row r="9" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1417,7 +1488,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickTop="1">
+    <row r="10" spans="1:3" ht="15.75" thickTop="1">
       <c r="A10" s="2" t="s">
         <v>85</v>
       </c>
@@ -1496,7 +1567,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -1512,8 +1583,8 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1"/>
-    <row r="22" spans="1:5" ht="16" thickTop="1" thickBot="1">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="22" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>10</v>
       </c>
@@ -1521,7 +1592,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" thickTop="1">
+    <row r="23" spans="1:5" ht="15.75" thickTop="1">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1529,7 +1600,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="14.5" customHeight="1">
+    <row r="24" spans="1:5" ht="14.45" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>75</v>
       </c>
@@ -1569,13 +1640,13 @@
         <v>-1497</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" thickBot="1"/>
-    <row r="30" spans="1:5" ht="16" thickTop="1" thickBot="1">
+    <row r="29" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="30" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
       <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" thickTop="1">
+    <row r="31" spans="1:5" ht="15.75" thickTop="1">
       <c r="A31" s="4" t="s">
         <v>63</v>
       </c>
@@ -1633,8 +1704,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15" thickBot="1"/>
-    <row r="39" spans="1:6" ht="16" thickTop="1" thickBot="1">
+    <row r="38" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="39" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A39" s="1" t="s">
         <v>69</v>
       </c>
@@ -1642,7 +1713,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15" thickTop="1">
+    <row r="40" spans="1:6" ht="15.75" thickTop="1">
       <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1652,8 +1723,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15" thickBot="1"/>
-    <row r="43" spans="1:6" ht="16" thickTop="1" thickBot="1">
+    <row r="42" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="43" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
@@ -1661,7 +1732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="43" thickTop="1">
+    <row r="44" spans="1:6" ht="60.75" thickTop="1">
       <c r="A44" s="4" t="s">
         <v>18</v>
       </c>
@@ -1686,13 +1757,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1"/>
-    <row r="48" spans="1:6" ht="16" thickTop="1" thickBot="1">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="48" spans="1:6" ht="16.5" thickTop="1" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" thickTop="1">
+    <row r="49" spans="1:2" ht="15.75" thickTop="1">
       <c r="A49" t="s">
         <v>87</v>
       </c>
@@ -1727,37 +1798,37 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickTop="1" thickBot="1">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2294,28 +2365,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="1" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -2323,7 +2394,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2365,7 +2436,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1">
+    <row r="3" spans="1:14" ht="15.75" thickTop="1">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2460,8 +2531,8 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1"/>
-    <row r="11" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="10" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="11" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -2469,7 +2540,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2551,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="13" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2491,7 +2562,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1">
+    <row r="14" spans="1:14" ht="15.75" thickBot="1">
       <c r="A14">
         <v>0.5</v>
       </c>
@@ -2502,7 +2573,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15">
         <v>1.5</v>
       </c>
@@ -2513,7 +2584,7 @@
         <v>0.87999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1">
       <c r="A16">
         <v>2.5</v>
       </c>
@@ -2524,7 +2595,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1">
       <c r="A17">
         <v>3.5000000000000004</v>
       </c>
@@ -2535,7 +2606,7 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1">
       <c r="A18">
         <v>4.5</v>
       </c>
@@ -2546,7 +2617,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1">
       <c r="A19">
         <v>5.5</v>
       </c>
@@ -2557,7 +2628,7 @@
         <v>1.4949999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1">
       <c r="A20">
         <v>6.5</v>
       </c>
@@ -2568,7 +2639,7 @@
         <v>3.3249999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1">
       <c r="A21">
         <v>7.5</v>
       </c>
@@ -2579,7 +2650,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1">
       <c r="A22">
         <v>8.5</v>
       </c>
@@ -2590,7 +2661,7 @@
         <v>1.5449999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1">
       <c r="A23">
         <v>9.5</v>
       </c>
@@ -2601,7 +2672,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
       <c r="A24">
         <v>10.5</v>
       </c>
@@ -2612,7 +2683,7 @@
         <v>1.5899999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
       <c r="A25">
         <v>11.5</v>
       </c>
@@ -2623,7 +2694,7 @@
         <v>1.84</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
       <c r="A26">
         <v>12.5</v>
       </c>
@@ -2634,7 +2705,7 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
       <c r="A27">
         <v>13.5</v>
       </c>
@@ -2645,7 +2716,7 @@
         <v>3.43</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
       <c r="A28">
         <v>14.499999999999998</v>
       </c>
@@ -2656,7 +2727,7 @@
         <v>4.79</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1">
       <c r="A29">
         <v>15.5</v>
       </c>
@@ -2667,7 +2738,7 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
       <c r="A30">
         <v>16.5</v>
       </c>
@@ -2678,7 +2749,7 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1">
       <c r="A31">
         <v>17.5</v>
       </c>
@@ -2689,7 +2760,7 @@
         <v>4.1549999999999994</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1">
       <c r="A32">
         <v>18.5</v>
       </c>
@@ -2700,7 +2771,7 @@
         <v>3.7850000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1">
       <c r="A33">
         <v>19.5</v>
       </c>
@@ -2711,7 +2782,7 @@
         <v>3.08</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1">
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
       <c r="A34">
         <v>20.5</v>
       </c>
@@ -2722,7 +2793,7 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
       <c r="A35">
         <v>21.5</v>
       </c>
@@ -2733,7 +2804,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
       <c r="A36">
         <v>22.5</v>
       </c>
@@ -2744,7 +2815,7 @@
         <v>4.4749999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
       <c r="A37">
         <v>23.5</v>
       </c>
@@ -2755,7 +2826,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1">
       <c r="A38">
         <v>24.5</v>
       </c>
@@ -2766,7 +2837,7 @@
         <v>4.04</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1">
+    <row r="39" spans="1:3" ht="15.75" thickBot="1">
       <c r="A39">
         <v>25.5</v>
       </c>
@@ -2777,7 +2848,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1">
       <c r="A40">
         <v>26.5</v>
       </c>
@@ -2788,7 +2859,7 @@
         <v>1.9849999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1">
       <c r="A41">
         <v>27.500000000000004</v>
       </c>
@@ -2799,7 +2870,7 @@
         <v>4.96</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1">
       <c r="A42">
         <v>28.499999999999996</v>
       </c>
@@ -2810,7 +2881,7 @@
         <v>2.2199999999999998</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1">
       <c r="A43">
         <v>29.5</v>
       </c>
@@ -2821,7 +2892,7 @@
         <v>3.3449999999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1">
       <c r="A44">
         <v>30.5</v>
       </c>
@@ -2832,7 +2903,7 @@
         <v>7.6849999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1">
+    <row r="45" spans="1:3" ht="15.75" thickBot="1">
       <c r="A45">
         <v>31.5</v>
       </c>
@@ -2843,7 +2914,7 @@
         <v>7.0449999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1">
+    <row r="46" spans="1:3" ht="15.75" thickBot="1">
       <c r="A46">
         <v>32.5</v>
       </c>
@@ -2854,7 +2925,7 @@
         <v>6.4449999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1">
+    <row r="47" spans="1:3" ht="15.75" thickBot="1">
       <c r="A47">
         <v>33.5</v>
       </c>
@@ -2865,7 +2936,7 @@
         <v>3.1549999999999998</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1">
+    <row r="48" spans="1:3" ht="15.75" thickBot="1">
       <c r="A48">
         <v>34.5</v>
       </c>
@@ -2876,7 +2947,7 @@
         <v>1.405</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1">
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
       <c r="A49">
         <v>35.5</v>
       </c>
@@ -2887,7 +2958,7 @@
         <v>2.0350000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" thickBot="1">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1">
       <c r="A50">
         <v>36.5</v>
       </c>
@@ -2898,7 +2969,7 @@
         <v>3.0950000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1">
+    <row r="51" spans="1:3" ht="15.75" thickBot="1">
       <c r="A51">
         <v>37.5</v>
       </c>
@@ -2909,7 +2980,7 @@
         <v>5.6449999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" thickBot="1">
+    <row r="52" spans="1:3" ht="15.75" thickBot="1">
       <c r="A52">
         <v>38.5</v>
       </c>
@@ -2920,7 +2991,7 @@
         <v>5.8149999999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1">
+    <row r="53" spans="1:3" ht="15.75" thickBot="1">
       <c r="A53">
         <v>39.5</v>
       </c>
@@ -2931,7 +3002,7 @@
         <v>4.5149999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1">
       <c r="A54">
         <v>40.5</v>
       </c>
@@ -2942,7 +3013,7 @@
         <v>2.04</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1">
+    <row r="55" spans="1:3" ht="15.75" thickBot="1">
       <c r="A55">
         <v>41.5</v>
       </c>
@@ -2953,7 +3024,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1">
       <c r="A56">
         <v>42.5</v>
       </c>
@@ -2964,7 +3035,7 @@
         <v>6.8550000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15" thickBot="1">
+    <row r="57" spans="1:3" ht="15.75" thickBot="1">
       <c r="A57">
         <v>43.5</v>
       </c>
@@ -2975,7 +3046,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1">
+    <row r="58" spans="1:3" ht="15.75" thickBot="1">
       <c r="A58">
         <v>44.5</v>
       </c>
@@ -2986,7 +3057,7 @@
         <v>7.4799999999999995</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" thickBot="1">
+    <row r="59" spans="1:3" ht="15.75" thickBot="1">
       <c r="A59">
         <v>45.5</v>
       </c>
@@ -2997,7 +3068,7 @@
         <v>4.5049999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" thickBot="1">
+    <row r="60" spans="1:3" ht="15.75" thickBot="1">
       <c r="A60">
         <v>46.5</v>
       </c>
@@ -3008,7 +3079,7 @@
         <v>4.26</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" thickBot="1">
+    <row r="61" spans="1:3" ht="15.75" thickBot="1">
       <c r="A61">
         <v>47.5</v>
       </c>
@@ -3019,7 +3090,7 @@
         <v>4.7549999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" thickBot="1">
+    <row r="62" spans="1:3" ht="15.75" thickBot="1">
       <c r="A62">
         <v>48.5</v>
       </c>
@@ -3041,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:A23"/>
   <sheetViews>
@@ -3049,7 +3120,7 @@
       <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="1:1">
       <c r="A3" s="7" t="s">
@@ -3166,27 +3237,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="3" max="3" width="45.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="1" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -3194,7 +3265,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="2" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
@@ -3236,7 +3307,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickTop="1">
+    <row r="3" spans="1:14" ht="15.75" thickTop="1">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -3372,8 +3443,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1"/>
-    <row r="12" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="12" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -3381,7 +3452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="13" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A13" s="16" t="s">
         <v>34</v>
       </c>
@@ -3392,7 +3463,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="16" thickTop="1" thickBot="1">
+    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
       <c r="A14" s="17" t="s">
         <v>99</v>
       </c>
@@ -3406,7 +3477,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15">
         <v>0.5</v>
       </c>
@@ -3420,7 +3491,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1">
       <c r="A16">
         <v>1.5</v>
       </c>
@@ -3434,7 +3505,7 @@
         <v>2.69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1">
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="A17">
         <v>2.5</v>
       </c>
@@ -3448,7 +3519,7 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1">
+    <row r="18" spans="1:4" ht="15.75" thickBot="1">
       <c r="A18">
         <v>3.5000000000000004</v>
       </c>
@@ -3462,7 +3533,7 @@
         <v>2.36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1">
+    <row r="19" spans="1:4" ht="15.75" thickBot="1">
       <c r="A19">
         <v>4.5</v>
       </c>
@@ -3476,7 +3547,7 @@
         <v>3.57</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1">
+    <row r="20" spans="1:4" ht="15.75" thickBot="1">
       <c r="A20">
         <v>5.5</v>
       </c>
@@ -3490,7 +3561,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1">
+    <row r="21" spans="1:4" ht="15.75" thickBot="1">
       <c r="A21">
         <v>6.5</v>
       </c>
@@ -3504,7 +3575,7 @@
         <v>5.56</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1">
       <c r="A22">
         <v>7.5</v>
       </c>
@@ -3518,7 +3589,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1">
       <c r="A23">
         <v>8.5</v>
       </c>
@@ -3532,7 +3603,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1">
       <c r="A24">
         <v>9.5</v>
       </c>
@@ -3546,7 +3617,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1">
       <c r="A25">
         <v>10.5</v>
       </c>
@@ -3560,7 +3631,7 @@
         <v>3.53</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1">
+    <row r="26" spans="1:4" ht="15.75" thickBot="1">
       <c r="A26">
         <v>11.5</v>
       </c>
@@ -3574,7 +3645,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1">
+    <row r="27" spans="1:4" ht="15.75" thickBot="1">
       <c r="A27">
         <v>12.5</v>
       </c>
@@ -3588,7 +3659,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1">
       <c r="A28">
         <v>13.5</v>
       </c>
@@ -3602,7 +3673,7 @@
         <v>5.87</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1">
       <c r="A29">
         <v>14.499999999999998</v>
       </c>
@@ -3616,7 +3687,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1">
       <c r="A30">
         <v>15.5</v>
       </c>
@@ -3630,7 +3701,7 @@
         <v>6.97</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1">
       <c r="A31">
         <v>16.5</v>
       </c>
@@ -3644,7 +3715,7 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1">
       <c r="A32">
         <v>17.5</v>
       </c>
@@ -3658,7 +3729,7 @@
         <v>6.31</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1">
       <c r="A33">
         <v>18.5</v>
       </c>
@@ -3672,7 +3743,7 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1">
       <c r="A34">
         <v>19.5</v>
       </c>
@@ -3686,7 +3757,7 @@
         <v>5.15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1">
       <c r="A35">
         <v>20.5</v>
       </c>
@@ -3700,7 +3771,7 @@
         <v>5.53</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1">
       <c r="A36">
         <v>21.5</v>
       </c>
@@ -3714,7 +3785,7 @@
         <v>3.67</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1">
       <c r="A37">
         <v>22.5</v>
       </c>
@@ -3728,7 +3799,7 @@
         <v>7.68</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1">
       <c r="A38">
         <v>23.5</v>
       </c>
@@ -3742,7 +3813,7 @@
         <v>3.14</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1">
       <c r="A39">
         <v>24.5</v>
       </c>
@@ -3756,7 +3827,7 @@
         <v>6.22</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1">
       <c r="A40">
         <v>25.5</v>
       </c>
@@ -3770,7 +3841,7 @@
         <v>5.92</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1">
       <c r="A41">
         <v>26.5</v>
       </c>
@@ -3784,7 +3855,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1">
       <c r="A42">
         <v>27.500000000000004</v>
       </c>
@@ -3798,7 +3869,7 @@
         <v>7.17</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
       <c r="A43">
         <v>28.499999999999996</v>
       </c>
@@ -3812,7 +3883,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
       <c r="A44">
         <v>29.5</v>
       </c>
@@ -3826,7 +3897,7 @@
         <v>5.35</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1">
       <c r="A45">
         <v>30.5</v>
       </c>
@@ -3840,7 +3911,7 @@
         <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
       <c r="A46">
         <v>31.5</v>
       </c>
@@ -3854,7 +3925,7 @@
         <v>9.27</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1">
       <c r="A47">
         <v>32.5</v>
       </c>
@@ -3868,7 +3939,7 @@
         <v>8.6199999999999992</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1">
       <c r="A48">
         <v>33.5</v>
       </c>
@@ -3882,7 +3953,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
       <c r="A49">
         <v>34.5</v>
       </c>
@@ -3896,7 +3967,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" thickBot="1">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1">
       <c r="A50">
         <v>35.5</v>
       </c>
@@ -3910,7 +3981,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" thickBot="1">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1">
       <c r="A51">
         <v>36.5</v>
       </c>
@@ -3924,7 +3995,7 @@
         <v>5.12</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" thickBot="1">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1">
       <c r="A52">
         <v>37.5</v>
       </c>
@@ -3938,7 +4009,7 @@
         <v>7.71</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" thickBot="1">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
       <c r="A53">
         <v>38.5</v>
       </c>
@@ -3952,7 +4023,7 @@
         <v>8.08</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" thickBot="1">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1">
       <c r="A54">
         <v>39.5</v>
       </c>
@@ -3966,7 +4037,7 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" thickBot="1">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1">
       <c r="A55">
         <v>40.5</v>
       </c>
@@ -3980,7 +4051,7 @@
         <v>3.59</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" thickBot="1">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1">
       <c r="A56">
         <v>41.5</v>
       </c>
@@ -3994,7 +4065,7 @@
         <v>4.76</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" thickBot="1">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1">
       <c r="A57">
         <v>42.5</v>
       </c>
@@ -4008,7 +4079,7 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" thickBot="1">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1">
       <c r="A58">
         <v>43.5</v>
       </c>
@@ -4022,7 +4093,7 @@
         <v>6.91</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1">
       <c r="A59">
         <v>44.5</v>
       </c>
@@ -4036,7 +4107,7 @@
         <v>9.61</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" thickBot="1">
+    <row r="60" spans="1:4" ht="15.75" thickBot="1">
       <c r="A60">
         <v>45.5</v>
       </c>
@@ -4050,7 +4121,7 @@
         <v>6.53</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1">
       <c r="A61">
         <v>46.5</v>
       </c>
@@ -4064,7 +4135,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1">
       <c r="A62">
         <v>47.5</v>
       </c>
@@ -4078,7 +4149,7 @@
         <v>6.72</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" thickBot="1">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1">
       <c r="A63">
         <v>48.5</v>
       </c>
@@ -4132,75 +4203,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>